<commit_message>
Created first pass of assembly drawing, drill drawing, and BOM in Microchip format.
</commit_message>
<xml_diff>
--- a/mini/v15/Fubarino_Mini_v15_BOM_SeeedFormat.xlsx
+++ b/mini/v15/Fubarino_Mini_v15_BOM_SeeedFormat.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\mini\v15\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="24615" windowHeight="9135" tabRatio="795"/>
   </bookViews>
@@ -561,7 +566,7 @@
     <definedName name="美金對美金" localSheetId="0">#REF!</definedName>
     <definedName name="美金對美金">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1048,9 +1053,6 @@
     <t>Radial through hole</t>
   </si>
   <si>
-    <t>V1.3</t>
-  </si>
-  <si>
     <t>Product Name：  Fubarino Mini</t>
   </si>
   <si>
@@ -1082,6 +1084,9 @@
   </si>
   <si>
     <t>C5, C13</t>
+  </si>
+  <si>
+    <t>V1.5</t>
   </si>
 </sst>
 </file>
@@ -2565,6 +2570,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -39258,7 +39266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39293,7 +39301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39510,7 +39518,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B19" sqref="B19"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="16.5"/>
@@ -39577,7 +39585,7 @@
     </row>
     <row r="6" spans="1:14" s="11" customFormat="1" ht="24.75" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="16"/>
@@ -39589,10 +39597,10 @@
     </row>
     <row r="7" spans="1:14" s="11" customFormat="1" ht="24.75" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -39760,7 +39768,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" s="51">
         <v>1</v>
@@ -39798,7 +39806,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="51">
         <v>1</v>
@@ -39836,7 +39844,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="51">
         <v>2</v>
@@ -40096,7 +40104,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="51">
         <v>3</v>
@@ -40147,19 +40155,19 @@
       </c>
       <c r="F25" s="33"/>
       <c r="G25" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H25" s="40" t="s">
         <v>88</v>
       </c>
       <c r="I25" s="74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J25" s="54" t="s">
         <v>82</v>
       </c>
       <c r="K25" s="74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
@@ -40215,7 +40223,7 @@
         <v>33</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
@@ -40384,7 +40392,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" s="32">
         <v>1</v>
@@ -40393,7 +40401,7 @@
         <v>86</v>
       </c>
       <c r="E33" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
@@ -41081,11 +41089,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="L10:L12"/>
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="K10:K12"/>
@@ -41098,6 +41101,11 @@
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="H10:H12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>